<commit_message>
Cambio imagen por atribuciones
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion02/SolicitudGrafica CN_09_02_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion02/SolicitudGrafica CN_09_02_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="205">
   <si>
     <t>Fecha:</t>
   </si>
@@ -625,9 +625,6 @@
   </si>
   <si>
     <t>Ilustración de un investigador con una cadena de ADN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/e/e8/Protein_alignment.jpg </t>
   </si>
   <si>
     <t>Secuencias de datos bioinformáticos</t>
@@ -649,7 +646,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -809,6 +806,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1359,7 +1362,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1582,6 +1585,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1680,9 +1686,7 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2423,8 +2427,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2470,14 +2474,14 @@
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="87"/>
+      <c r="F2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="80"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2501,14 +2505,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="87">
+      <c r="C3" s="88">
         <v>9</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="F3" s="80">
+      <c r="D3" s="89"/>
+      <c r="F3" s="81">
         <v>42241</v>
       </c>
-      <c r="G3" s="81"/>
+      <c r="G3" s="82"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2532,10 +2536,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2564,10 +2568,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2649,12 +2653,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -2758,7 +2762,7 @@
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="78" t="s">
         <v>193</v>
       </c>
       <c r="C11" s="20" t="str">
@@ -2927,13 +2931,13 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
-      <c r="B15" s="62" t="s">
-        <v>201</v>
+      <c r="B15" s="110">
+        <v>73145722</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -2962,7 +2966,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
@@ -3005,7 +3009,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
@@ -3019,7 +3023,7 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3048,7 +3052,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K17" s="66"/>
       <c r="O17" s="2" t="str">
@@ -5980,25 +5984,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -6006,11 +6010,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6061,11 +6065,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="105" t="str">
+      <c r="D5" s="106" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6110,12 +6114,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="91" t="str">
+      <c r="D7" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6209,14 +6213,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="95"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6249,12 +6253,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="99"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6294,12 +6298,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="99" t="str">
+      <c r="D17" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="102"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6315,12 +6319,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="91" t="str">
+      <c r="D18" s="92" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -6711,40 +6715,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="109" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="108" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="107"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>